<commit_message>
Add redirect to contagion_content study
</commit_message>
<xml_diff>
--- a/setup/Clues.xlsx
+++ b/setup/Clues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameshoughton/Google Drive/MIT PhD/Factionalism_Research/detective-game-interdependent-diffusion/setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4A43FD-6107-B84F-BFE4-CC346AF5FF09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F6EA70-4FF6-B64F-8054-2E2D11CAC919}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14920" yWindow="-19500" windowWidth="28800" windowHeight="17540" xr2:uid="{B21006E5-5609-314C-A9D2-507389E26D8D}"/>
   </bookViews>
@@ -8419,6 +8419,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8669,14 +8677,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9017,7 +9017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D17421D-7336-214C-8C21-6BC5BECB8A53}">
   <dimension ref="A1:AJ299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -14780,7 +14780,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B79">
-    <cfRule type="duplicateValues" dxfId="16" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14790,7 +14790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04637A0D-6076-A04A-90B7-1BB318B0C9C2}">
   <dimension ref="A1:F735"/>
   <sheetViews>
-    <sheetView topLeftCell="A509" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+    <sheetView topLeftCell="A513" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
       <selection activeCell="D541" sqref="D541"/>
     </sheetView>
   </sheetViews>
@@ -29850,10 +29850,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F735">
-    <cfRule type="duplicateValues" dxfId="15" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37249,55 +37249,55 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D53:D67">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",D53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",D53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="found">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="found">
       <formula>NOT(ISERROR(SEARCH("found",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53:D67">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="owns">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="owns">
       <formula>NOT(ISERROR(SEARCH("owns",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183:D198">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",D183)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",D183)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="found">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="found">
       <formula>NOT(ISERROR(SEARCH("found",D183)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183:D198">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="owns">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="owns">
       <formula>NOT(ISERROR(SEARCH("owns",D183)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D200:D215">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",D200)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",D200)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="found">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="found">
       <formula>NOT(ISERROR(SEARCH("found",D200)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D200:D215">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="owns">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="owns">
       <formula>NOT(ISERROR(SEARCH("owns",D200)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F262:F293">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46762,7 +46762,7 @@
   </sheetData>
   <autoFilter ref="E1:E201" xr:uid="{9253C666-B95B-CD47-9A24-3FA88CDD763D}">
     <filterColumn colId="0">
-      <colorFilter dxfId="26"/>
+      <colorFilter dxfId="1"/>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E1:E1048576">
@@ -47173,17 +47173,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:N13">
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="found">
+    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="found">
       <formula>NOT(ISERROR(SEARCH("found",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:N14">
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:N13">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="owns">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="owns">
       <formula>NOT(ISERROR(SEARCH("owns",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47571,28 +47571,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B8">
-    <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="found">
+    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="found">
       <formula>NOT(ISERROR(SEARCH("found",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B8">
-    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:H8 B2:N3">
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="seen">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="seen">
       <formula>NOT(ISERROR(SEARCH("seen",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="5" operator="containsText" text="found">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="found">
       <formula>NOT(ISERROR(SEARCH("found",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:H8 A2:N3">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="owns">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="owns">
       <formula>NOT(ISERROR(SEARCH("owns",A2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>